<commit_message>
changes according for new proj
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurusaishreeshtirumalla/Dropbox/My Mac (gurusaishreesh-MBP.local)/Desktop/Emailbot_apk/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurusaishreeshtirumalla/Desktop/pyproj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AD90BF-5DCE-7848-AF44-95F0710B9284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F9A71A2-C263-E947-A8B1-D62F396DB0DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{36E2957E-6CDE-3C4D-9373-6583AB28DC48}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{36E2957E-6CDE-3C4D-9373-6583AB28DC48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>SNO</t>
   </si>
@@ -48,10 +48,13 @@
     <t>guru.sai.shreesh@gmail.com</t>
   </si>
   <si>
-    <t>komal mam</t>
-  </si>
-  <si>
-    <t>komalkaur13@gmail.com</t>
+    <t>alekhya</t>
+  </si>
+  <si>
+    <t>nishita mam</t>
+  </si>
+  <si>
+    <t>alekhyakanjarla@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF498152-080F-3245-96A7-5BCBEAE97C4E}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,14 +470,26 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{85D7A331-49F1-7A45-A91D-D7DBB4AB1BA0}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{6F9EA0E3-1BD4-A348-A5A0-8F9940F028C5}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{2E14E758-1596-8C47-8E2C-E57921D00DE3}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{9A4786B4-F0F3-444C-8F6A-205D36652944}"/>
+    <hyperlink ref="C4" r:id="rId4" display="gojo.testing123@gmail.com" xr:uid="{98DF030E-00B4-3B4E-B556-373C63892DC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>